<commit_message>
Re-Upload with correct Directory Structure
</commit_message>
<xml_diff>
--- a/admin/receiving/register-inbound/file_uploads/Essentials Case Goods Invoice No. 0026.15 - Container No. TCLU 595703-5, BL ITJ7019677 (1) (2).xlsx
+++ b/admin/receiving/register-inbound/file_uploads/Essentials Case Goods Invoice No. 0026.15 - Container No. TCLU 595703-5, BL ITJ7019677 (1) (2).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssAlien\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27792" windowHeight="12528"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,19 +489,19 @@
     <t>Invoice No. 026/15 - Essentials Case Goods  Line - B/L No.ITJ7019677</t>
   </si>
   <si>
-    <t>Container No. TCLU 595703-5</t>
-  </si>
-  <si>
     <t>VSL - MCS BARBARA</t>
   </si>
   <si>
-    <t>ETA Lexington 10/23/2015</t>
+    <t>Container No. TCLU 595334-1</t>
+  </si>
+  <si>
+    <t>ETA Lexington 12/14/2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -623,6 +628,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -670,7 +678,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -705,7 +713,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -917,37 +925,37 @@
   <dimension ref="A1:C144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
     <col min="2" max="2" width="76" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -958,7 +966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>4151</v>
       </c>
@@ -969,7 +977,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>4152</v>
       </c>
@@ -980,7 +988,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>4153</v>
       </c>
@@ -991,7 +999,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>4141</v>
       </c>
@@ -1002,7 +1010,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>4142</v>
       </c>
@@ -1013,7 +1021,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>4143</v>
       </c>
@@ -1024,7 +1032,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>4171</v>
       </c>
@@ -1035,7 +1043,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>4172</v>
       </c>
@@ -1046,7 +1054,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>4173</v>
       </c>
@@ -1057,7 +1065,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>4181</v>
       </c>
@@ -1068,7 +1076,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>4182</v>
       </c>
@@ -1079,7 +1087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>4183</v>
       </c>
@@ -1090,7 +1098,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>4191</v>
       </c>
@@ -1101,7 +1109,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>4192</v>
       </c>
@@ -1112,7 +1120,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>4193</v>
       </c>
@@ -1123,7 +1131,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>41101</v>
       </c>
@@ -1134,7 +1142,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>41102</v>
       </c>
@@ -1145,7 +1153,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>41103</v>
       </c>
@@ -1156,7 +1164,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>41111</v>
       </c>
@@ -1167,7 +1175,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>41112</v>
       </c>
@@ -1178,7 +1186,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>41113</v>
       </c>
@@ -1189,10 +1197,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>4143</v>
       </c>
@@ -1203,10 +1211,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C32" s="9"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>148</v>
       </c>
@@ -1217,12 +1225,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>10</v>
       </c>
@@ -1233,7 +1241,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>11</v>
       </c>
@@ -1244,7 +1252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>12</v>
       </c>
@@ -1255,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>16</v>
       </c>
@@ -1266,7 +1274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>17</v>
       </c>
@@ -1277,7 +1285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -1288,7 +1296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>22</v>
       </c>
@@ -1299,7 +1307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>23</v>
       </c>
@@ -1310,7 +1318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>24</v>
       </c>
@@ -1321,7 +1329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>28</v>
       </c>
@@ -1332,7 +1340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>29</v>
       </c>
@@ -1343,7 +1351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>30</v>
       </c>
@@ -1354,7 +1362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>40</v>
       </c>
@@ -1365,7 +1373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>41</v>
       </c>
@@ -1376,7 +1384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>42</v>
       </c>
@@ -1387,7 +1395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>37</v>
       </c>
@@ -1398,7 +1406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>38</v>
       </c>
@@ -1409,7 +1417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>39</v>
       </c>
@@ -1420,7 +1428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>46</v>
       </c>
@@ -1431,7 +1439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>47</v>
       </c>
@@ -1442,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>48</v>
       </c>
@@ -1453,7 +1461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>52</v>
       </c>
@@ -1464,7 +1472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>53</v>
       </c>
@@ -1475,7 +1483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>54</v>
       </c>
@@ -1486,7 +1494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>58</v>
       </c>
@@ -1497,7 +1505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>59</v>
       </c>
@@ -1508,7 +1516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>60</v>
       </c>
@@ -1519,7 +1527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>64</v>
       </c>
@@ -1530,7 +1538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>65</v>
       </c>
@@ -1541,7 +1549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>66</v>
       </c>
@@ -1552,7 +1560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>70</v>
       </c>
@@ -1563,7 +1571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>71</v>
       </c>
@@ -1574,7 +1582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>72</v>
       </c>
@@ -1585,7 +1593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>76</v>
       </c>
@@ -1596,7 +1604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>77</v>
       </c>
@@ -1607,7 +1615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>78</v>
       </c>
@@ -1618,7 +1626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>82</v>
       </c>
@@ -1629,7 +1637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>83</v>
       </c>
@@ -1640,7 +1648,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>84</v>
       </c>
@@ -1651,7 +1659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>88</v>
       </c>
@@ -1662,7 +1670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>89</v>
       </c>
@@ -1673,7 +1681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>90</v>
       </c>
@@ -1684,7 +1692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>94</v>
       </c>
@@ -1695,7 +1703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>95</v>
       </c>
@@ -1706,7 +1714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>96</v>
       </c>
@@ -1717,7 +1725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>100</v>
       </c>
@@ -1728,7 +1736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>101</v>
       </c>
@@ -1739,7 +1747,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>102</v>
       </c>
@@ -1750,7 +1758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>106</v>
       </c>
@@ -1761,7 +1769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>107</v>
       </c>
@@ -1772,7 +1780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>108</v>
       </c>
@@ -1783,7 +1791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>112</v>
       </c>
@@ -1794,7 +1802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>113</v>
       </c>
@@ -1805,7 +1813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>114</v>
       </c>
@@ -1816,12 +1824,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B127" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>4151</v>
       </c>
@@ -1832,7 +1840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>4152</v>
       </c>
@@ -1843,7 +1851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>4153</v>
       </c>
@@ -1854,7 +1862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>4131</v>
       </c>
@@ -1865,7 +1873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>4132</v>
       </c>
@@ -1876,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>4133</v>
       </c>
@@ -1887,7 +1895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>4141</v>
       </c>
@@ -1898,7 +1906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>4142</v>
       </c>
@@ -1909,7 +1917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>4143</v>
       </c>
@@ -1920,7 +1928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>4161</v>
       </c>
@@ -1931,7 +1939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>4162</v>
       </c>
@@ -1942,7 +1950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>4163</v>
       </c>
@@ -1953,7 +1961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>131</v>
       </c>
@@ -1970,7 +1978,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1982,7 +1990,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>